<commit_message>
add title, change styling
</commit_message>
<xml_diff>
--- a/scatter_plot/aggregated.xlsx
+++ b/scatter_plot/aggregated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82946c1d38922a58/我的文档/课程资料/INFO5100/project3/code/scatter_plot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:40009_{8E40BA00-E5A5-D14A-A29D-98919921F503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1E7E17E-BA4F-684B-9161-E41C63280C4E}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:40009_{8E40BA00-E5A5-D14A-A29D-98919921F503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{262A182C-D8CF-B047-844C-D98B38EBBE02}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1554,7 +1554,7 @@
   <dimension ref="A1:M814"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A189" sqref="A189"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34808,8 +34808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L159"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>